<commit_message>
manuscript V3 and production table
</commit_message>
<xml_diff>
--- a/manuscript/meso_tx_table.xlsx
+++ b/manuscript/meso_tx_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="540" windowWidth="17540" windowHeight="10820" tabRatio="257"/>
+    <workbookView xWindow="1180" yWindow="0" windowWidth="20600" windowHeight="15160" tabRatio="257"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -54,6 +54,27 @@
   </si>
   <si>
     <t>ave meso</t>
+  </si>
+  <si>
+    <t>daily average division rate</t>
+  </si>
+  <si>
+    <t>daily average crypto</t>
+  </si>
+  <si>
+    <t>daily average production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>M. major abundance (10^6 cells/L)</t>
+  </si>
+  <si>
+    <t>average daily cryptophyte production (10^6 cells/L*day)</t>
   </si>
 </sst>
 </file>
@@ -64,9 +85,25 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -89,18 +126,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,14 +495,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="11" width="11" style="3" customWidth="1"/>
@@ -829,9 +897,342 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1">
+        <v>41529</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="1">
+        <v>41530</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1">
+        <v>41533</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="D24" s="6">
+        <v>42624</v>
+      </c>
+      <c r="E24">
+        <v>0.53</v>
+      </c>
+      <c r="F24">
+        <v>0.193</v>
+      </c>
+      <c r="G24">
+        <f>E24*F24</f>
+        <v>0.10229000000000001</v>
+      </c>
+      <c r="H24">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1">
+        <v>41534</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="D25" s="6">
+        <v>42625</v>
+      </c>
+      <c r="E25">
+        <v>1.49</v>
+      </c>
+      <c r="F25">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" ref="G25:G31" si="1">E25*F25</f>
+        <v>8.0907000000000007E-2</v>
+      </c>
+      <c r="H25">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1">
+        <v>41536</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="D26" s="6">
+        <v>42630</v>
+      </c>
+      <c r="E26">
+        <v>1.28</v>
+      </c>
+      <c r="F26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H26">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1">
+        <v>41537</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="D27" s="6">
+        <v>42636</v>
+      </c>
+      <c r="E27">
+        <v>0.59</v>
+      </c>
+      <c r="F27">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="1"/>
+        <v>9.8530000000000006E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1">
+        <v>41540</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="D28" s="6">
+        <v>42637</v>
+      </c>
+      <c r="E28">
+        <v>0.3</v>
+      </c>
+      <c r="F28">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="1"/>
+        <v>1.95E-2</v>
+      </c>
+      <c r="H28">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="1">
+        <v>41541</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="D29" s="6">
+        <v>42638</v>
+      </c>
+      <c r="E29">
+        <v>0.37</v>
+      </c>
+      <c r="F29">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0320000000000004E-2</v>
+      </c>
+      <c r="H29">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="1">
+        <v>41542</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="D30" s="6">
+        <v>42639</v>
+      </c>
+      <c r="E30">
+        <v>0.23</v>
+      </c>
+      <c r="F30">
+        <v>9.5699999999999993E-2</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2010999999999999E-2</v>
+      </c>
+      <c r="H30">
+        <v>9.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1">
+        <v>41543</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="D31" s="6">
+        <v>42644</v>
+      </c>
+      <c r="E31">
+        <v>0.9</v>
+      </c>
+      <c r="F31">
+        <v>0.183</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="1"/>
+        <v>0.16470000000000001</v>
+      </c>
+      <c r="H31">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="1">
+        <v>41544</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>41547</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>41548</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>41549</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>41550</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="48">
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="E38" s="7">
+        <v>41528</v>
+      </c>
+      <c r="F38">
+        <v>0.1</v>
+      </c>
+      <c r="G38">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="E39" s="7">
+        <v>41529</v>
+      </c>
+      <c r="F39">
+        <v>0.08</v>
+      </c>
+      <c r="G39">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="E40" s="7">
+        <v>41534</v>
+      </c>
+      <c r="F40">
+        <v>0.03</v>
+      </c>
+      <c r="G40">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="E41" s="7">
+        <v>41540</v>
+      </c>
+      <c r="F41">
+        <v>0.09</v>
+      </c>
+      <c r="G41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="E42" s="7">
+        <v>41541</v>
+      </c>
+      <c r="F42">
+        <v>0.02</v>
+      </c>
+      <c r="G42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="E43" s="7">
+        <v>41542</v>
+      </c>
+      <c r="F43">
+        <v>0.05</v>
+      </c>
+      <c r="G43">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" s="7">
+        <v>41543</v>
+      </c>
+      <c r="F44">
+        <v>0.02</v>
+      </c>
+      <c r="G44">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="E45" s="7">
+        <v>41548</v>
+      </c>
+      <c r="F45">
+        <v>0.16</v>
+      </c>
+      <c r="G45">
+        <v>0.08</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -850,7 +1251,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -872,7 +1273,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>